<commit_message>
Fix: silhouette persistence and date-based game state management
</commit_message>
<xml_diff>
--- a/euroleague_2025-2026_roster_photos.xlsx
+++ b/euroleague_2025-2026_roster_photos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kayrakocagil/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kayrakocagil/Documents/mirsad-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FCCA061-54E2-604B-8237-A384F1156213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4E0BD0-6B6A-DE42-B3DC-9E793318E7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2839,11 +2839,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H346"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A314" workbookViewId="0">
+      <selection activeCell="A344" activeCellId="12" sqref="A19:A20 A55:A56 A92:A93 A129:A130 A144:A145 A182:A183 A211:A212 A244:A245 A262 A281 A303 A321 A344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>